<commit_message>
Complete calculate score, fix bug
</commit_message>
<xml_diff>
--- a/websitetesttoeic.frontend/public/LuanVan_Demo/Excel.xlsx
+++ b/websitetesttoeic.frontend/public/LuanVan_Demo/Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ty\websitetesttoeic.frontend\public\LuanVan_Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822E08BC-1C02-4A14-8E58-AA43148D4A2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1664E1BC-3A87-47CB-B1A4-142E8D8C7AC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>ContentAnswer</t>
   </si>
@@ -361,7 +361,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:L10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -544,9 +544,7 @@
       <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>